<commit_message>
Add 2^k results & analysis
</commit_message>
<xml_diff>
--- a/jupyter/cifar10-2k.xlsx
+++ b/jupyter/cifar10-2k.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\abe\fltk-testbed\jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF9FFD6-4B39-4E77-886A-F6CBB626ACDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02216FA-2A62-40E4-9EC5-233AAF159683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AvgProcessorUtil" sheetId="1" r:id="rId1"/>
-    <sheet name="AvgTrainTime" sheetId="3" r:id="rId2"/>
-    <sheet name="AvgAccuracy" sheetId="4" r:id="rId3"/>
+    <sheet name="AvgAccuracy" sheetId="4" r:id="rId1"/>
+    <sheet name="AvgProcessorUtil" sheetId="1" r:id="rId2"/>
+    <sheet name="AvgTrainTime" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -428,11 +428,594 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC886D8-5C88-45FC-AA5B-C5C06F807112}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>56.792999999999999</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>56.792999999999999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>60.356999999999999</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60.356999999999999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>57.37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>57.37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>61.128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>61.128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>56.792999999999999</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>56.792999999999999</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>60.356999999999999</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>60.356999999999999</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>57.37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>57.37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>61.128</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>61.128</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>47.88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>47.88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>52.024000000000001</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>52.024000000000001</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40.64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>40.64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>44.52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>44.52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>47.88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>47.88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>52.024000000000001</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>52.024000000000001</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40.64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40.64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>44.52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>44.52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +1044,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>26.5</v>
+      </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -475,6 +1061,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>26.5</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -489,6 +1078,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>26.52</v>
+      </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -503,6 +1095,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>26.5</v>
+      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -517,6 +1112,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>26.5</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -531,6 +1129,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>26.5</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -545,6 +1146,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>26.5</v>
+      </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -559,6 +1163,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>26.5</v>
+      </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -573,6 +1180,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50.5</v>
+      </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -587,6 +1197,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50.5</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -601,6 +1214,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50.558999999999997</v>
+      </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -615,6 +1231,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50.5</v>
+      </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -629,6 +1248,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>49.2</v>
+      </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -643,6 +1265,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>49.332999999999998</v>
+      </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -657,6 +1282,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>49.42</v>
+      </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -670,7 +1298,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>49.238999999999997</v>
+      </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -684,7 +1315,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>26.664000000000001</v>
+      </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -698,7 +1332,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>26.364000000000001</v>
+      </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -712,7 +1349,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>26.04</v>
+      </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -726,7 +1366,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>26.356000000000002</v>
+      </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -740,7 +1383,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>24.064</v>
+      </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -754,7 +1400,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24.664000000000001</v>
+      </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -768,7 +1417,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25.58</v>
+      </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -782,7 +1434,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25.295999999999999</v>
+      </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -796,7 +1451,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>49.131999999999998</v>
+      </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -810,7 +1468,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>48.963999999999999</v>
+      </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -824,7 +1485,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>49.94</v>
+      </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -838,7 +1502,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>49.835999999999999</v>
+      </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -852,7 +1519,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>48.295999999999999</v>
+      </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
@@ -866,7 +1536,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>44.531999999999996</v>
+      </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -880,7 +1553,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>47.72</v>
+      </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
@@ -894,7 +1570,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>44.54</v>
+      </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -910,15 +1589,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D708A7-956E-4361-BDCB-ACF575AB70D5}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,6 +1627,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>795882.33299999998</v>
+      </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -961,6 +1644,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>788823</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -975,6 +1661,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1196585.8</v>
+      </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -989,6 +1678,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1187479.3999999999</v>
+      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1003,6 +1695,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>801656.33299999998</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1017,6 +1712,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>758754.33299999998</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1031,6 +1729,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1193829.2</v>
+      </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1045,6 +1746,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1179058.3999999999</v>
+      </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1059,6 +1763,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>378391.33299999998</v>
+      </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -1073,6 +1780,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>379282</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -1087,6 +1797,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>583195</v>
+      </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -1101,6 +1814,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>574298.4</v>
+      </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -1115,6 +1831,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>370748.66600000003</v>
+      </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -1129,6 +1848,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>395633</v>
+      </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -1143,6 +1865,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>581766.80000000005</v>
+      </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -1156,7 +1881,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>578386</v>
+      </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1898,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>219991</v>
+      </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1915,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>206888.33300000001</v>
+      </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1198,7 +1932,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>312384.2</v>
+      </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1212,7 +1949,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>314543.59999999998</v>
+      </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -1226,7 +1966,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>214427</v>
+      </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +1983,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>206381</v>
+      </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +2000,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>326699.59999999998</v>
+      </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -1268,7 +2017,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>320761.2</v>
+      </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -1282,7 +2034,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>102110.333</v>
+      </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +2051,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>101938</v>
+      </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +2068,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>153616.79999999999</v>
+      </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +2085,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>154355.4</v>
+      </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +2102,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>106975.333</v>
+      </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
@@ -1352,7 +2119,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>109180.666</v>
+      </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1366,7 +2136,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>158281.4</v>
+      </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
@@ -1380,493 +2153,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC886D8-5C88-45FC-AA5B-C5C06F807112}">
-  <dimension ref="A1:E33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>158150.6</v>
+      </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>

</xml_diff>